<commit_message>
add complete function to gpw module; create main
</commit_message>
<xml_diff>
--- a/today_date_error_logs.xlsx
+++ b/today_date_error_logs.xlsx
@@ -14,18 +14,129 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>./D_data/1/2021-07-27.xls</t>
-  </si>
-  <si>
-    <t>./D_data/1/2021-07-30.xls</t>
-  </si>
-  <si>
-    <t>./D_data/1/2021-07-28.xls</t>
-  </si>
-  <si>
-    <t>./D_data/1/2021-07-29.xls</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+  <si>
+    <t>./D_data/1/2019-12-24.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2020-01-01.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2020-04-10.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-17.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-30.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-09.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2020-12-24.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2020-04-13.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-12-31.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-27.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2020-12-31.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-11.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-04-19.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-10.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-08-15.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-19.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-26.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-06-03.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-06-20.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-18.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-12-26.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-05-03.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-25.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2020-05-01.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-05-01.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-31.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-05-03.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-01-06.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-20.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-23.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-12-25.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-01-01.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-04-22.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-04-02.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-16.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-24.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-12.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2020-12-25.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-04-05.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2019-01-01.xls</t>
+  </si>
+  <si>
+    <t>./D_data/1/2021-08-13.xls</t>
   </si>
 </sst>
 </file>
@@ -383,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,6 +537,302 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>